<commit_message>
Simulo todos los escenarios por 25 anios
</commit_message>
<xml_diff>
--- a/static/resultados.xlsx
+++ b/static/resultados.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezemati\Downloads\Projects\simulacion-tp6\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842E4D1D-B275-4E09-94C3-D309B7C7F74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4141DF17-700B-4298-BBD8-A2500C601CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20240916_110044" sheetId="1" r:id="rId1"/>
     <sheet name="20240923_135227" sheetId="2" r:id="rId2"/>
+    <sheet name="20240928_034311" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>CANT_JUNIORS</t>
   </si>
@@ -162,19 +163,120 @@
   </si>
   <si>
     <t>92.01005659208639  ,  91.65688398055329  ,  91.98594789453873  ,  91.45331961197289</t>
+  </si>
+  <si>
+    <t>0.494</t>
+  </si>
+  <si>
+    <t>41.094</t>
+  </si>
+  <si>
+    <t>36.038  ,  36.038</t>
+  </si>
+  <si>
+    <t>67.704</t>
+  </si>
+  <si>
+    <t>57.317  ,  57.317  ,  57.317</t>
+  </si>
+  <si>
+    <t>67.903</t>
+  </si>
+  <si>
+    <t>68.015  ,  68.016  ,  68.015  ,  68.015</t>
+  </si>
+  <si>
+    <t>67.854</t>
+  </si>
+  <si>
+    <t>0.663</t>
+  </si>
+  <si>
+    <t>69.7  ,  69.7</t>
+  </si>
+  <si>
+    <t>36.155  ,  36.155</t>
+  </si>
+  <si>
+    <t>83.885  ,  83.885</t>
+  </si>
+  <si>
+    <t>57.368  ,  57.368  ,  57.368</t>
+  </si>
+  <si>
+    <t>83.918  ,  83.919</t>
+  </si>
+  <si>
+    <t>67.995  ,  67.995  ,  67.995  ,  67.995</t>
+  </si>
+  <si>
+    <t>83.894  ,  83.894</t>
+  </si>
+  <si>
+    <t>0.681</t>
+  </si>
+  <si>
+    <t>79.756  ,  79.757  ,  79.757</t>
+  </si>
+  <si>
+    <t>36.166  ,  36.166</t>
+  </si>
+  <si>
+    <t>89.259  ,  89.259  ,  89.26</t>
+  </si>
+  <si>
+    <t>57.381  ,  57.382  ,  57.381</t>
+  </si>
+  <si>
+    <t>89.28  ,  89.284  ,  89.286</t>
+  </si>
+  <si>
+    <t>68.084  ,  68.085  ,  68.085  ,  68.085</t>
+  </si>
+  <si>
+    <t>89.281  ,  89.275  ,  89.282</t>
+  </si>
+  <si>
+    <t>0.688</t>
+  </si>
+  <si>
+    <t>84.806  ,  84.806  ,  84.806  ,  84.806</t>
+  </si>
+  <si>
+    <t>36.052  ,  36.052</t>
+  </si>
+  <si>
+    <t>91.906  ,  91.906  ,  91.906  ,  91.91</t>
+  </si>
+  <si>
+    <t>57.343  ,  57.343  ,  57.343</t>
+  </si>
+  <si>
+    <t>91.952  ,  91.952  ,  91.944  ,  91.95</t>
+  </si>
+  <si>
+    <t>67.974  ,  67.974  ,  67.973  ,  67.974</t>
+  </si>
+  <si>
+    <t>91.941  ,  91.836  ,  91.941  ,  91.936</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -195,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -233,16 +335,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -960,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1090,4 +1210,415 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2847.8789999999999</v>
+      </c>
+      <c r="D2">
+        <v>271.81400000000002</v>
+      </c>
+      <c r="E2">
+        <v>1.284</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>213.64699999999999</v>
+      </c>
+      <c r="D3">
+        <v>150.59299999999999</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>30.364999999999998</v>
+      </c>
+      <c r="D4">
+        <v>148.16900000000001</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5.3940000000000001</v>
+      </c>
+      <c r="D5">
+        <v>148.08699999999999</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2405.08</v>
+      </c>
+      <c r="D6">
+        <v>31.021000000000001</v>
+      </c>
+      <c r="E6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>212.21299999999999</v>
+      </c>
+      <c r="D7">
+        <v>8.5609999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>30.210999999999999</v>
+      </c>
+      <c r="D8">
+        <v>8.5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>5.4139999999999997</v>
+      </c>
+      <c r="D9">
+        <v>8.5890000000000004</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>2350.0450000000001</v>
+      </c>
+      <c r="D10">
+        <v>5.3979999999999997</v>
+      </c>
+      <c r="E10">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>211.83500000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>30.158000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>5.3109999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2337.9839999999999</v>
+      </c>
+      <c r="D14">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>212.51499999999999</v>
+      </c>
+      <c r="D15">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>30.565000000000001</v>
+      </c>
+      <c r="D16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>5.4480000000000004</v>
+      </c>
+      <c r="D17">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>